<commit_message>
sign in module includes signin,firsttimewrongOTP,signintwowindows,signindataset,invalidsignin4times,invalidsignin5times,invalidsignintwobrowsers
</commit_message>
<xml_diff>
--- a/InputFiles/Web/Suite_Web.xlsx
+++ b/InputFiles/Web/Suite_Web.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="23320" windowHeight="13220"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="23320" windowHeight="13240"/>
   </bookViews>
   <sheets>
     <sheet name="Suite" sheetId="1" r:id="rId1"/>
@@ -84,13 +84,14 @@
     <t>N</t>
   </si>
   <si>
-    <t>NEW_MESSAGE-1</t>
-  </si>
-  <si>
     <t>COMPOSEMESSAGE</t>
   </si>
   <si>
     <t>Y</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SIGNIN</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -976,7 +977,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -1134,13 +1135,14 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>21</v>
-      </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>